<commit_message>
updated watering and ferti logs
</commit_message>
<xml_diff>
--- a/logs/hoagland_ph_weekly_mk.xlsx
+++ b/logs/hoagland_ph_weekly_mk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mrkel\Documents\git\2025_g34p\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09B6276-3424-4F82-860B-C3756EB62357}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A50B8A2B-94AC-4C8A-B117-8B2EF6559D0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
+    <workbookView xWindow="14565" yWindow="465" windowWidth="12480" windowHeight="13035" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>hoagland solution fertilizer weekly pH</t>
   </si>
@@ -72,12 +72,6 @@
   </si>
   <si>
     <t>week 05</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*Overfilled by 675 mL on 08/15/2025. pH was 6.87, corrected by adding extra nut. On 08/18/2025, new pH. </t>
   </si>
 </sst>
 </file>
@@ -119,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E599DF-0674-4691-8FF2-730716D2E8B0}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,6 +509,12 @@
       <c r="C6">
         <v>6.37</v>
       </c>
+      <c r="D6" s="2">
+        <v>6.36</v>
+      </c>
+      <c r="E6">
+        <v>6.61</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -525,6 +526,12 @@
       <c r="C7">
         <v>7.01</v>
       </c>
+      <c r="D7" s="2">
+        <v>6.79</v>
+      </c>
+      <c r="E7">
+        <v>6.79</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -536,6 +543,12 @@
       <c r="C8">
         <v>6.96</v>
       </c>
+      <c r="D8" s="2">
+        <v>7.01</v>
+      </c>
+      <c r="E8">
+        <v>6.74</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -547,13 +560,11 @@
       <c r="C9">
         <v>6.54</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
+      <c r="D9" s="2">
+        <v>6.21</v>
+      </c>
+      <c r="E9">
+        <v>6.46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
li600 data upload, added script to check li_600 MIA data
</commit_message>
<xml_diff>
--- a/logs/hoagland_ph_weekly_mk.xlsx
+++ b/logs/hoagland_ph_weekly_mk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monik\Documents\git\2025_g34p\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B262277-13FD-45CF-BAC7-8BE32993AA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB17AF1B-E991-46EA-842B-9F49401BC3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13776" xr2:uid="{8D8DBED7-4830-46A9-B76D-E0096B6445E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -456,21 +456,21 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="14.88671875" customWidth="1"/>
+    <col min="2" max="7" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -478,10 +478,27 @@
         <v>45880</v>
       </c>
       <c r="C4" s="1">
-        <v>45884</v>
+        <f>B4+7</f>
+        <v>45887</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4:G4" si="0">C4+7</f>
+        <v>45894</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="0"/>
+        <v>45901</v>
+      </c>
+      <c r="F4" s="1">
+        <f t="shared" si="0"/>
+        <v>45908</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>45915</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -504,7 +521,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -527,7 +544,7 @@
         <v>6.26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -550,7 +567,7 @@
         <v>6.91</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -573,7 +590,7 @@
         <v>6.79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>4</v>
       </c>

</xml_diff>